<commit_message>
Adding New Screening Data
</commit_message>
<xml_diff>
--- a/Data/E_Cigarette_Data.xlsx
+++ b/Data/E_Cigarette_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/reuben_frost_icr_ac_uk/Documents/Documents/UK-cancer-trends/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{1D65AEFD-6684-4FCF-A2FA-955FC68E945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F58494C2-CF80-49CD-AFE8-310B50337716}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{1D65AEFD-6684-4FCF-A2FA-955FC68E945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66839F77-D545-4BFE-AF1C-C29612AA471B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="8" activeTab="12" xr2:uid="{22ADE637-891C-44EC-B9E0-E01E3C7DDF77}"/>
   </bookViews>
@@ -27,6 +27,9 @@
     <sheet name="NIreland_All" sheetId="12" r:id="rId12"/>
     <sheet name="Great_Britain_All" sheetId="13" r:id="rId13"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Great_Britain_All!$A$1:$T$19</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1007,9 +1010,12 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="54" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="87">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2863,25 +2869,39 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C664E547-6A6D-44D2-8B91-69DF058D9FFB}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E1" t="s">
@@ -2896,7 +2916,7 @@
       <c r="H1" t="s">
         <v>78</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>79</v>
       </c>
       <c r="J1" t="s">
@@ -2929,7 +2949,7 @@
       <c r="S1" t="s">
         <v>89</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3057,7 +3077,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -3119,7 +3139,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -3181,7 +3201,7 @@
         <v>85.2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -3243,7 +3263,7 @@
         <v>52350</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -3429,7 +3449,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -3491,7 +3511,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -3553,7 +3573,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -3615,7 +3635,7 @@
         <v>52321</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -3801,7 +3821,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -3863,7 +3883,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -3925,7 +3945,7 @@
         <v>85.8</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2020</v>
       </c>
@@ -3987,7 +4007,7 @@
         <v>52103</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2020</v>
       </c>
@@ -4050,6 +4070,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:T19" xr:uid="{C664E547-6A6D-44D2-8B91-69DF058D9FFB}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Daily user (%)"/>
+        <filter val="Occasional user (%)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Removing datapoint in Position Paper graphs
Datapoint from age_group merging removed due to concerns with the weighted bases for that year
</commit_message>
<xml_diff>
--- a/Data/E_Cigarette_Data.xlsx
+++ b/Data/E_Cigarette_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/reuben_frost_icr_ac_uk/Documents/Documents/UK-cancer-trends/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{1D65AEFD-6684-4FCF-A2FA-955FC68E945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66839F77-D545-4BFE-AF1C-C29612AA471B}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="8_{1D65AEFD-6684-4FCF-A2FA-955FC68E945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8510EEB3-3685-41A3-946C-38A85F00BB1C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="8" activeTab="12" xr2:uid="{22ADE637-891C-44EC-B9E0-E01E3C7DDF77}"/>
   </bookViews>
@@ -2869,11 +2869,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C664E547-6A6D-44D2-8B91-69DF058D9FFB}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3077,7 +3076,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -3139,7 +3138,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -3201,7 +3200,7 @@
         <v>85.2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -3263,7 +3262,7 @@
         <v>52350</v>
       </c>
     </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -3449,7 +3448,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -3511,7 +3510,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -3573,7 +3572,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -3635,7 +3634,7 @@
         <v>52321</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -3821,7 +3820,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -3883,7 +3882,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -3945,7 +3944,7 @@
         <v>85.8</v>
       </c>
     </row>
-    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2020</v>
       </c>
@@ -4007,7 +4006,7 @@
         <v>52103</v>
       </c>
     </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2020</v>
       </c>
@@ -4070,14 +4069,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T19" xr:uid="{C664E547-6A6D-44D2-8B91-69DF058D9FFB}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Daily user (%)"/>
-        <filter val="Occasional user (%)"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>